<commit_message>
convert lat lon diffrence to x y in meters and get distance between 2 points
</commit_message>
<xml_diff>
--- a/carstop.xlsx
+++ b/carstop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Faculty\GP\Graduation-Project-V2V\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C96381E-CC18-4E7B-8E4E-DA582D8B8F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D983529E-4F8A-49DD-AA58-09678703441E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="138">
   <si>
     <t>Column1</t>
   </si>
@@ -97,12 +97,6 @@
     <t>Column16</t>
   </si>
   <si>
-    <t>Column17</t>
-  </si>
-  <si>
-    <t>Column18</t>
-  </si>
-  <si>
     <t>{'vecid':</t>
   </si>
   <si>
@@ -142,9 +136,6 @@
     <t>'angle':</t>
   </si>
   <si>
-    <t>12.116777931556612}</t>
-  </si>
-  <si>
     <t>31.347866761322827,</t>
   </si>
   <si>
@@ -160,9 +151,6 @@
     <t>1.5987136533925745e-06,</t>
   </si>
   <si>
-    <t>360.0}</t>
-  </si>
-  <si>
     <t>31.347851523043936,</t>
   </si>
   <si>
@@ -223,9 +211,6 @@
     <t>1.4384213268510548e-06,</t>
   </si>
   <si>
-    <t>90.00279799132335}</t>
-  </si>
-  <si>
     <t>31.347778923596636,</t>
   </si>
   <si>
@@ -328,9 +313,6 @@
     <t>8.934547462419779e-07,</t>
   </si>
   <si>
-    <t>269.99720200867665}</t>
-  </si>
-  <si>
     <t>31.347804177549953,</t>
   </si>
   <si>
@@ -473,6 +455,12 @@
   </si>
   <si>
     <t>locationy2</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>anglesa</t>
   </si>
 </sst>
 </file>
@@ -643,12 +631,12 @@
     <tableColumn id="14" xr3:uid="{8A06A901-1A72-457B-9C88-81E5A8FFA389}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="5"/>
     <tableColumn id="15" xr3:uid="{A70CECE6-59B4-4299-B566-C4719D6953DD}" uniqueName="15" name="Column15" queryTableFieldId="15" dataDxfId="4"/>
     <tableColumn id="16" xr3:uid="{C43270D4-D147-47A9-8C29-5A2040C2A238}" uniqueName="16" name="Column16" queryTableFieldId="16"/>
-    <tableColumn id="17" xr3:uid="{739546DD-70BF-426D-973E-8A882ECC991A}" uniqueName="17" name="Column17" queryTableFieldId="17" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{DA91B2BF-DA2B-44EC-886B-1903B8C1998B}" uniqueName="18" name="Column18" queryTableFieldId="18" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{CA76202F-8D6D-4B8F-92E2-E590CBA190C8}" uniqueName="19" name="locationx2" queryTableFieldId="19" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{739546DD-70BF-426D-973E-8A882ECC991A}" uniqueName="17" name="anglesa" queryTableFieldId="17" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{DA91B2BF-DA2B-44EC-886B-1903B8C1998B}" uniqueName="18" name="angle" queryTableFieldId="18" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{CA76202F-8D6D-4B8F-92E2-E590CBA190C8}" uniqueName="19" name="locationx2" queryTableFieldId="19" dataDxfId="1">
       <calculatedColumnFormula>LEFT(F2, LEN(F2)-2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{5C58AC76-04C9-4786-8E4E-AC1867C0DEAE}" uniqueName="20" name="locationy2" queryTableFieldId="20" dataDxfId="1">
+    <tableColumn id="20" xr3:uid="{5C58AC76-04C9-4786-8E4E-AC1867C0DEAE}" uniqueName="20" name="locationy2" queryTableFieldId="20" dataDxfId="0">
       <calculatedColumnFormula>LEFT(H2, LEN(H2)-2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -922,7 +910,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,16 +982,16 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
+        <v>137</v>
       </c>
       <c r="R1" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="S1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="T1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -1014,52 +1002,52 @@
         <v>0.87944305555555558</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>242606374551181</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="R2" s="3">
+        <v>12.1167779315566</v>
       </c>
       <c r="S2" s="3" t="str">
         <f t="shared" ref="S2:S23" si="0">LEFT(F2, LEN(F2)-2)</f>
@@ -1078,52 +1066,52 @@
         <v>0.87947788194444443</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>242606374551181</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="M3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R3" s="3">
+        <v>360</v>
       </c>
       <c r="S3" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1142,52 +1130,52 @@
         <v>0.87951263888888886</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>242606374551181</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R4" s="3">
+        <v>360</v>
       </c>
       <c r="S4" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1206,52 +1194,52 @@
         <v>0.87954721064814811</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>242606374551181</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="H5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R5" s="3">
+        <v>360</v>
       </c>
       <c r="S5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1270,52 +1258,52 @@
         <v>0.87958199074074073</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>242606374551181</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="H6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="M6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R6" s="3">
+        <v>360</v>
       </c>
       <c r="S6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1334,52 +1322,52 @@
         <v>0.87961692129629632</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>242606374551181</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="H7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="M7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>58</v>
+        <v>28</v>
+      </c>
+      <c r="R7" s="3">
+        <v>90.002797991323305</v>
       </c>
       <c r="S7" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1398,52 +1386,52 @@
         <v>0.87965136574074076</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>242606374551181</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R8" s="3">
+        <v>360</v>
       </c>
       <c r="S8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1462,52 +1450,52 @@
         <v>0.87968655092592596</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>242606374551181</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O9" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R9" s="3">
+        <v>360</v>
       </c>
       <c r="S9" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1526,52 +1514,52 @@
         <v>0.87972106481481482</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>242606374551181</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R10" s="3">
+        <v>360</v>
       </c>
       <c r="S10" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1590,52 +1578,52 @@
         <v>0.8797558680555555</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>242606374551181</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="K11" s="3" t="s">
+      <c r="L11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M11" s="3" t="s">
+      <c r="N11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P11">
         <v>0</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R11" s="3">
+        <v>360</v>
       </c>
       <c r="S11" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1654,52 +1642,52 @@
         <v>0.87979027777777774</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>242606374551181</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="J12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K12" s="3" t="s">
+      <c r="L12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="M12" s="3" t="s">
+      <c r="N12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O12" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P12">
         <v>0</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R12" s="3">
+        <v>360</v>
       </c>
       <c r="S12" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1718,52 +1706,52 @@
         <v>0.87982525462962968</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D13">
         <v>242606374551181</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="I13" s="3" t="s">
+      <c r="J13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K13" s="3" t="s">
+      <c r="L13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L13" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="M13" s="3" t="s">
+      <c r="N13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O13" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P13">
         <v>0</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R13" s="3">
+        <v>360</v>
       </c>
       <c r="S13" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1782,52 +1770,52 @@
         <v>0.879859849537037</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14">
         <v>242606374551181</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="J14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K14" s="3" t="s">
+      <c r="L14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="M14" s="3" t="s">
+      <c r="N14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="O14" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P14">
         <v>0</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R14" s="3" t="s">
-        <v>93</v>
+        <v>28</v>
+      </c>
+      <c r="R14" s="3">
+        <v>269.99720200867603</v>
       </c>
       <c r="S14" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1846,52 +1834,52 @@
         <v>0.87989464120370375</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15">
         <v>242606374551181</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I15" s="3" t="s">
+      <c r="J15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="K15" s="3" t="s">
+      <c r="L15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L15" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="M15" s="3" t="s">
+      <c r="N15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O15" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R15" s="3">
+        <v>360</v>
       </c>
       <c r="S15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1910,52 +1898,52 @@
         <v>0.87992986111111116</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16">
         <v>242606374551181</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="I16" s="3" t="s">
+      <c r="J16" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="K16" s="3" t="s">
+      <c r="L16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="M16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L16" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="M16" s="3" t="s">
+      <c r="N16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="O16" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R16" s="3">
+        <v>360</v>
       </c>
       <c r="S16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1974,52 +1962,52 @@
         <v>0.87996409722222224</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D17">
         <v>242606374551181</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I17" s="3" t="s">
+      <c r="J17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="K17" s="3" t="s">
+      <c r="L17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L17" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M17" s="3" t="s">
+      <c r="N17" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="O17" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P17">
         <v>0</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R17" s="3">
+        <v>360</v>
       </c>
       <c r="S17" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2038,52 +2026,52 @@
         <v>0.87999902777777783</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>242606374551181</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I18" s="3" t="s">
+      <c r="J18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M18" s="3" t="s">
+      <c r="N18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O18" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P18">
         <v>0</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R18" s="3">
+        <v>360</v>
       </c>
       <c r="S18" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2102,52 +2090,52 @@
         <v>0.88003355324074073</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <v>242606374551181</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L19" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="M19" s="3" t="s">
+      <c r="N19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="O19" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P19">
         <v>0</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R19" s="3">
+        <v>360</v>
       </c>
       <c r="S19" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2166,52 +2154,52 @@
         <v>0.88006825231481478</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20">
         <v>242606374551181</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="I20" s="3" t="s">
+      <c r="J20" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="K20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="K20" s="3" t="s">
+      <c r="L20" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L20" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="M20" s="3" t="s">
+      <c r="N20" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P20">
         <v>0</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R20" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R20" s="3">
+        <v>360</v>
       </c>
       <c r="S20" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2230,52 +2218,52 @@
         <v>0.88010322916666661</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D21">
         <v>242606374551181</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="I21" s="3" t="s">
+      <c r="J21" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="K21" s="3" t="s">
+      <c r="L21" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="M21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L21" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="M21" s="3" t="s">
+      <c r="N21" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="O21" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P21">
         <v>0</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R21" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R21" s="3">
+        <v>360</v>
       </c>
       <c r="S21" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2294,52 +2282,52 @@
         <v>0.88013759259259261</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D22">
         <v>242606374551181</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I22" s="3" t="s">
+      <c r="J22" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="K22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J22" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="K22" s="3" t="s">
+      <c r="L22" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="M22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L22" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="M22" s="3" t="s">
+      <c r="N22" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="O22" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P22">
         <v>0</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R22" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R22" s="3">
+        <v>360</v>
       </c>
       <c r="S22" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2358,52 +2346,52 @@
         <v>0.88017243055555561</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D23">
         <v>242606374551181</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="I23" s="3" t="s">
+      <c r="J23" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="K23" s="3" t="s">
+      <c r="L23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="M23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L23" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="M23" s="3" t="s">
+      <c r="N23" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="O23" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="P23">
         <v>0</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R23" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="R23" s="3">
+        <v>360</v>
       </c>
       <c r="S23" s="3" t="str">
         <f t="shared" si="0"/>

</xml_diff>